<commit_message>
Lang code changed from spa to es
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_category.xlsx
+++ b/mosip_master/xlsx/doc_category.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="doc_category" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">doc_category!$A$1:$K$27</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="71">
   <si>
     <t>code</t>
   </si>
@@ -44,6 +47,24 @@
     <t>is_active</t>
   </si>
   <si>
+    <t>cr_by</t>
+  </si>
+  <si>
+    <t>cr_dtimes</t>
+  </si>
+  <si>
+    <t>upd_by</t>
+  </si>
+  <si>
+    <t>upd_dtimes</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
+  </si>
+  <si>
+    <t>del_dtimes</t>
+  </si>
+  <si>
     <t>POA</t>
   </si>
   <si>
@@ -56,6 +77,45 @@
     <t>eng</t>
   </si>
   <si>
+    <t>rediet</t>
+  </si>
+  <si>
+    <t>masterdata-220005</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Un justificatif de domicile</t>
+  </si>
+  <si>
+    <t>Preuve dadresse</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>ganesh</t>
+  </si>
+  <si>
+    <t>पते का प्रमाण</t>
+  </si>
+  <si>
+    <t>निवास प्रमाण पत्र</t>
+  </si>
+  <si>
+    <t>hin</t>
+  </si>
+  <si>
+    <t>Comprobante de domicilio</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>spa_admin</t>
+  </si>
+  <si>
     <t>POI</t>
   </si>
   <si>
@@ -71,13 +131,34 @@
     <t>Proof of Relationship</t>
   </si>
   <si>
-    <t>पते का प्रमाण</t>
-  </si>
-  <si>
-    <t>निवास प्रमाण पत्र</t>
-  </si>
-  <si>
-    <t>hin</t>
+    <t>chithara</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>Proof of Consent</t>
+  </si>
+  <si>
+    <t>POE</t>
+  </si>
+  <si>
+    <t>Proof of Biometric Exception</t>
+  </si>
+  <si>
+    <t>chithara27</t>
+  </si>
+  <si>
+    <t>Preuve didentité</t>
+  </si>
+  <si>
+    <t>Preuve de relation</t>
+  </si>
+  <si>
+    <t>Preuve de relation de la personne</t>
+  </si>
+  <si>
+    <t>Preuve dexception biométrique</t>
   </si>
   <si>
     <t>सबूत की पहचान</t>
@@ -89,19 +170,7 @@
     <t>रिश्ते का सबूत</t>
   </si>
   <si>
-    <t>DocTestCode321</t>
-  </si>
-  <si>
-    <t>दॊच्चत्</t>
-  </si>
-  <si>
-    <t>दॊच्तॆस्त्चॊदॆ३२१ उप्दतॆद्</t>
-  </si>
-  <si>
-    <t>DocTestCode123</t>
-  </si>
-  <si>
-    <t>तॆस्तिन्ग् पॊसितिवॆ दॊच् उप्दतॆद्</t>
+    <t>बायोमेट्रिक अपवाद का प्रमाण</t>
   </si>
   <si>
     <t>POP</t>
@@ -113,121 +182,67 @@
     <t>Proof of Resident Photo</t>
   </si>
   <si>
-    <t>POE</t>
-  </si>
-  <si>
-    <t>बायोमेट्रिक अपवाद का प्रमाण</t>
-  </si>
-  <si>
-    <t>Proof of Biometric Exception</t>
+    <t>Prueba de identidad</t>
+  </si>
+  <si>
+    <t>Prueba de relación</t>
+  </si>
+  <si>
+    <t>Prueba de excepción biométrica</t>
+  </si>
+  <si>
+    <t>Prueba de consentimiento</t>
+  </si>
+  <si>
+    <t>Foto de residente</t>
+  </si>
+  <si>
+    <t>Prueba de foto de residente</t>
+  </si>
+  <si>
+    <t>POF</t>
+  </si>
+  <si>
+    <t>Proof Of Foreigner</t>
+  </si>
+  <si>
+    <t>Proof of Foreigner Identity</t>
+  </si>
+  <si>
+    <t>globaladmin</t>
+  </si>
+  <si>
+    <t>Proof of Foreigner</t>
   </si>
   <si>
     <t>POB</t>
   </si>
   <si>
+    <t>Preuve de naissance</t>
+  </si>
+  <si>
+    <t>Preuve de la date de naissance de la personne</t>
+  </si>
+  <si>
+    <t>Prueba de nacimiento</t>
+  </si>
+  <si>
+    <t>Prueba de fecha de nacimiento de la persona.</t>
+  </si>
+  <si>
+    <t>जन्म का प्रमाण</t>
+  </si>
+  <si>
+    <t>व्यक्ति के जन्म की तारीख का प्रमाण</t>
+  </si>
+  <si>
     <t>Proof of Birth</t>
   </si>
   <si>
     <t>Proof date of birth of the person</t>
   </si>
   <si>
-    <t>जन्म का प्रमाण</t>
-  </si>
-  <si>
-    <t>व्यक्ति के जन्म की तारीख का प्रमाण</t>
-  </si>
-  <si>
-    <t>POF</t>
-  </si>
-  <si>
-    <t>Proof Of Foreigner</t>
-  </si>
-  <si>
-    <t>Proof of Foreigner Identity</t>
-  </si>
-  <si>
-    <t>POC</t>
-  </si>
-  <si>
-    <t>Proof of Consent</t>
-  </si>
-  <si>
-    <t>Comprobante de domicilio</t>
-  </si>
-  <si>
-    <t>Comprobante de dirección</t>
-  </si>
-  <si>
-    <t>spa</t>
-  </si>
-  <si>
-    <t>Documentos de identidad</t>
-  </si>
-  <si>
-    <t>Prueba de identidad</t>
-  </si>
-  <si>
-    <t>Prueba de relación</t>
-  </si>
-  <si>
-    <t>Prueba de consentimiento</t>
-  </si>
-  <si>
-    <t>Prueba de excepción biométrica</t>
-  </si>
-  <si>
-    <t>Prueba de nacimiento</t>
-  </si>
-  <si>
-    <t>Prueba de fecha de nacimiento del persona</t>
-  </si>
-  <si>
-    <t>Foto residente</t>
-  </si>
-  <si>
-    <t>Foto de prueba de residente</t>
-  </si>
-  <si>
-    <t>Prueba de extranjero</t>
-  </si>
-  <si>
-    <t>Prueba de Identidad de Extranjero</t>
-  </si>
-  <si>
-    <t>Preuve d'adresse</t>
-  </si>
-  <si>
-    <t>fra</t>
-  </si>
-  <si>
-    <t>Preuve d'identité</t>
-  </si>
-  <si>
-    <t>Preuve de relation</t>
-  </si>
-  <si>
-    <t>Preuve de consentement</t>
-  </si>
-  <si>
-    <t>Preuve d'exception biométrique</t>
-  </si>
-  <si>
-    <t>Preuve de naissance</t>
-  </si>
-  <si>
-    <t>Preuve de la date de naissance de la personne</t>
-  </si>
-  <si>
-    <t>Photo du résident</t>
-  </si>
-  <si>
-    <t>Preuve de photo de résidence</t>
-  </si>
-  <si>
-    <t>Preuve d'étranger</t>
-  </si>
-  <si>
-    <t>Preuve d'identité étrangère</t>
+    <t>vishal</t>
   </si>
 </sst>
 </file>
@@ -843,14 +858,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1386,20 +1398,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="16.1818181818182" customWidth="1"/>
-    <col min="2" max="2" width="31.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="39.8181818181818" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1415,579 +1422,939 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44776.3535428286</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45663.2517515086</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="F3"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44960.3609410832</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>45663.2517515086</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="F4"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45005.5672956281</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1">
+        <v>45663.2517515086</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
-      <c r="F5"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>45663.2517515086</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
-      <c r="F6"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44776.3535428286</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
-      <c r="F7"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44776.3535428286</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1">
+        <v>44806.2610978022</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1103</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44811.7207822317</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1">
+        <v>44831.3902988818</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44776.3535428286</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="1">
+        <v>44853.2754040037</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="b">
+      <c r="G10" s="1">
+        <v>44960.3609410832</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="b">
         <v>1</v>
       </c>
-      <c r="F8"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G11" s="1">
+        <v>44960.3609410832</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44960.3609410832</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="b">
+      <c r="E13" t="b">
         <v>1</v>
       </c>
-      <c r="F9"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10" s="1"/>
-      <c r="H10"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11" s="1"/>
-      <c r="H11"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12"/>
-      <c r="G12" s="1"/>
-      <c r="H12"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13"/>
-      <c r="G13" s="1"/>
-      <c r="H13"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45005.5672956281</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14"/>
-      <c r="G14" s="1"/>
-      <c r="H14"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45005.5672956281</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45005.5672956281</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44791.5322257916</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1">
+        <v>45141.5398774277</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="1">
+        <v>44806.2610978009</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H19" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15" s="1"/>
-      <c r="H15"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="b">
+      <c r="I19" s="1">
+        <v>44853.2754040046</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="1">
+        <v>44831.3902988773</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="1">
+        <v>44811.2735578009</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="b">
         <v>1</v>
       </c>
-      <c r="F16"/>
-      <c r="G16" s="1"/>
-      <c r="H16"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="2" t="b">
+      <c r="F22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="1">
+        <v>45266.3452722103</v>
+      </c>
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="1">
+        <v>45266.3458456789</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="F23" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="G23" s="1">
+        <v>45266.3452748818</v>
+      </c>
+      <c r="H23" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="2" t="s">
+      <c r="I23" s="1">
+        <v>45266.3458456789</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="1">
+        <v>44960.3609410832</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="1">
+        <v>45637.2789113305</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="C25" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="1">
+        <v>44959.5260991081</v>
+      </c>
+      <c r="H25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="1">
+        <v>45637.2789113305</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="2" t="b">
-        <v>1</v>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45005.5672956281</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="1">
+        <v>45637.3188345087</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1">
+        <v>44776.3535428286</v>
+      </c>
+      <c r="H27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="1">
+        <v>45637.3196029031</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:K27" etc:filterBottomFollowUsedRange="0">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>